<commit_message>
updated code, readme, payments
</commit_message>
<xml_diff>
--- a/team-managment/purchases/project-payments .xlsx
+++ b/team-managment/purchases/project-payments .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhdgh\OneDrive\Desktop\on-campus-delivery-robot\team-managment\purchases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADB9E06-5B15-48CA-BB3F-CD4ACA84E515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEDAB2F-C8BC-491D-95E3-90C6E8AAB71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>ITEM</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>servo motor</t>
+  </si>
+  <si>
+    <t>Payment settled</t>
   </si>
 </sst>
 </file>
@@ -914,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ1006"/>
+  <dimension ref="A1:AMJ1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2110,24 +2113,24 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B29" s="10">
-        <v>6.24</v>
+        <v>133.35249999999999</v>
       </c>
       <c r="C29" s="10">
         <v>1</v>
       </c>
       <c r="D29" s="6">
-        <v>0</v>
+        <v>-133.35249999999999</v>
       </c>
       <c r="E29" s="6">
         <v>0</v>
       </c>
       <c r="F29" s="7">
-        <v>6.24</v>
+        <v>133.35249999999999</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -2154,10 +2157,10 @@
     </row>
     <row r="30" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B30" s="10">
-        <v>13</v>
+        <v>6.24</v>
       </c>
       <c r="C30" s="10">
         <v>1</v>
@@ -2166,10 +2169,10 @@
         <v>0</v>
       </c>
       <c r="E30" s="6">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F30" s="7">
-        <v>0</v>
+        <v>6.24</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -2195,22 +2198,23 @@
       <c r="AB30" s="2"/>
     </row>
     <row r="31" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>27</v>
+      <c r="A31" s="11" t="s">
+        <v>26</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14">
-        <f>SUM(D3:D30)</f>
-        <v>1460.2375</v>
+      <c r="B31" s="10">
+        <v>13</v>
       </c>
-      <c r="E31" s="14">
-        <f>SUM(E3:E30)</f>
-        <v>453</v>
+      <c r="C31" s="10">
+        <v>1</v>
       </c>
-      <c r="F31" s="15">
-        <f>SUM(F3:F30)</f>
-        <v>756.58999999999992</v>
+      <c r="D31" s="6">
+        <v>0</v>
+      </c>
+      <c r="E31" s="6">
+        <v>13</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -2236,22 +2240,22 @@
       <c r="AB31" s="2"/>
     </row>
     <row r="32" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>28</v>
+      <c r="A32" s="12" t="s">
+        <v>27</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18">
-        <f>SUM(E3:F30)/3</f>
-        <v>403.19666666666666</v>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14">
+        <f>SUM(D3:D31)</f>
+        <v>1326.885</v>
       </c>
-      <c r="E32" s="18">
-        <f>SUM(D3:D30,F3:F30)/3</f>
-        <v>738.9425</v>
+      <c r="E32" s="14">
+        <f>SUM(E3:E31)</f>
+        <v>453</v>
       </c>
-      <c r="F32" s="19">
-        <f>SUM(D3:E30)/3</f>
-        <v>637.74583333333328</v>
+      <c r="F32" s="15">
+        <f>SUM(F3:F31)</f>
+        <v>889.94249999999988</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2277,22 +2281,22 @@
       <c r="AB32" s="2"/>
     </row>
     <row r="33" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
-        <v>29</v>
+      <c r="A33" s="16" t="s">
+        <v>28</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="22">
-        <f>D32-2*D31/3</f>
-        <v>-570.29500000000007</v>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="18">
+        <f>SUM(E3:F31)/3</f>
+        <v>447.64749999999998</v>
       </c>
-      <c r="E33" s="22">
-        <f>E32-2*E31/3</f>
-        <v>436.9425</v>
+      <c r="E33" s="18">
+        <f>SUM(D3:D31,F3:F31)/3</f>
+        <v>738.94249999999977</v>
       </c>
-      <c r="F33" s="23">
-        <f>F32-2*F31/3</f>
-        <v>133.35250000000002</v>
+      <c r="F33" s="19">
+        <f>SUM(D3:E31)/3</f>
+        <v>593.29499999999996</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -2318,12 +2322,23 @@
       <c r="AB33" s="2"/>
     </row>
     <row r="34" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="A34" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22">
+        <f>D33-2*D32/3</f>
+        <v>-436.94250000000005</v>
+      </c>
+      <c r="E34" s="22">
+        <f>E33-2*E32/3</f>
+        <v>436.94249999999977</v>
+      </c>
+      <c r="F34" s="23">
+        <f>F33-2*F32/3</f>
+        <v>0</v>
+      </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -31507,6 +31522,36 @@
       <c r="AA1006" s="2"/>
       <c r="AB1006" s="2"/>
     </row>
+    <row r="1007" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1007" s="2"/>
+      <c r="B1007" s="2"/>
+      <c r="C1007" s="2"/>
+      <c r="D1007" s="2"/>
+      <c r="E1007" s="2"/>
+      <c r="F1007" s="2"/>
+      <c r="G1007" s="2"/>
+      <c r="H1007" s="2"/>
+      <c r="I1007" s="2"/>
+      <c r="J1007" s="2"/>
+      <c r="K1007" s="2"/>
+      <c r="L1007" s="2"/>
+      <c r="M1007" s="2"/>
+      <c r="N1007" s="2"/>
+      <c r="O1007" s="2"/>
+      <c r="P1007" s="2"/>
+      <c r="Q1007" s="2"/>
+      <c r="R1007" s="2"/>
+      <c r="S1007" s="2"/>
+      <c r="T1007" s="2"/>
+      <c r="U1007" s="2"/>
+      <c r="V1007" s="2"/>
+      <c r="W1007" s="2"/>
+      <c r="X1007" s="2"/>
+      <c r="Y1007" s="2"/>
+      <c r="Z1007" s="2"/>
+      <c r="AA1007" s="2"/>
+      <c r="AB1007" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>

</xml_diff>